<commit_message>
tweaked template and published
</commit_message>
<xml_diff>
--- a/Data/ReportTemplate.xlsx
+++ b/Data/ReportTemplate.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UiPath Projects\ListUSAPrivateSchools\ListUSAPrivateSchools_Producer\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UiPath Projects\ListUSAPrivateSchools\ListUSAPrivateSchools_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{364FAC97-9420-4414-9B4C-EC64E421839B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59BAD8B1-57E8-4170-B723-2EE1405CE4FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E07FBAE3-D5D4-4977-911A-2D0D075A38A4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E07FBAE3-D5D4-4977-911A-2D0D075A38A4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="SchoolsData" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>School Name</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>Phone number</t>
+  </si>
+  <si>
+    <t>Error Comment</t>
   </si>
 </sst>
 </file>
@@ -424,20 +427,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95AC3111-D238-4B0C-89FE-F33B70313DBD}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" customWidth="1"/>
-    <col min="2" max="2" width="29.44140625" customWidth="1"/>
-    <col min="5" max="5" width="15.77734375" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -452,6 +456,9 @@
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>